<commit_message>
modify window in AILabxTest2_3.py
</commit_message>
<xml_diff>
--- a/SRC/BackTest/data/AILabxTest2_3_info_2.xlsx
+++ b/SRC/BackTest/data/AILabxTest2_3_info_2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>pnl_ratio</t>
   </si>
@@ -55,6 +55,12 @@
   <si>
     <t>w_dd</t>
   </si>
+  <si>
+    <t>trend_score(close,25)*0.05+(roc(close,5)+roc(close,10))*0.05+ma(volume,5)/ma(volume,20)</t>
+  </si>
+  <si>
+    <t>roc(close, 21)&gt; 0.18</t>
+  </si>
 </sst>
 </file>
 
@@ -66,7 +72,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,13 +83,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -551,148 +550,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1047,13 +1046,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.8888888888889" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -1086,7 +1085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>3.21592328947339</v>
       </c>
@@ -1111,8 +1110,11 @@
       <c r="H2">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>3.19651786680629</v>
       </c>
@@ -1136,6 +1138,9 @@
       </c>
       <c r="H3">
         <v>0.18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3688,7 +3693,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H101">
-    <sortState ref="A2:H101">
+    <sortState ref="A1:H101">
       <sortCondition ref="A2" descending="1"/>
     </sortState>
     <extLst/>

</xml_diff>